<commit_message>
course bug(elective, mechanical major) fix
</commit_message>
<xml_diff>
--- a/edited/elective_list/hus.xlsx
+++ b/edited/elective_list/hus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GIST_Credit_Analysis_Program\edited\elective_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D3ABC4-6456-4CCB-BFA1-AC4670EC9F6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE8D1EA-BBA2-4B85-B1EE-A0714EC37BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="3324" windowWidth="11460" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="141">
   <si>
     <t>교과목</t>
   </si>
@@ -465,6 +465,10 @@
   </si>
   <si>
     <t>상품의 역사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GS2515</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -901,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D374"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1105,7 +1109,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>140</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1114,12 +1118,12 @@
         <v>2021</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>140</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -1128,12 +1132,12 @@
         <v>2021</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -1142,12 +1146,12 @@
         <v>2021</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1156,12 +1160,12 @@
         <v>2021</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -1170,12 +1174,12 @@
         <v>2021</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1184,12 +1188,12 @@
         <v>2021</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -1198,12 +1202,12 @@
         <v>2021</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1212,12 +1216,12 @@
         <v>2021</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1226,12 +1230,12 @@
         <v>2021</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1240,12 +1244,12 @@
         <v>2021</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1254,12 +1258,12 @@
         <v>2021</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -1268,12 +1272,12 @@
         <v>2021</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1282,12 +1286,12 @@
         <v>2021</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1296,12 +1300,12 @@
         <v>2021</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -1310,12 +1314,12 @@
         <v>2021</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -1324,12 +1328,12 @@
         <v>2021</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -1338,7 +1342,7 @@
         <v>2021</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>